<commit_message>
Coding part is completed now
</commit_message>
<xml_diff>
--- a/name.xlsx
+++ b/name.xlsx
@@ -14,6 +14,7 @@
     <sheet name="20thAug, 2021" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="31thAug, 2021" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="03thSep, 2021" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="11thSep, 2021" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -22,9 +23,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -1563,4 +1565,73 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="8" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>BARKAT</t>
+        </is>
+      </c>
+      <c r="B2" s="8" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="C2" s="10" t="n">
+        <v>44450.87703130787</v>
+      </c>
+      <c r="D2" s="10" t="n">
+        <v>44450.87708763889</v>
+      </c>
+      <c r="E2" s="10" t="n">
+        <v>44450.87713575231</v>
+      </c>
+      <c r="F2" s="10" t="n">
+        <v>44450.87718730697</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="8" t="inlineStr">
+        <is>
+          <t>Matching(%)</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>57.38756673793869</v>
+      </c>
+      <c r="D3" t="n">
+        <v>56.41789086541215</v>
+      </c>
+      <c r="E3" t="n">
+        <v>54.25104163473586</v>
+      </c>
+      <c r="F3" t="n">
+        <v>51.08050264201491</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>